<commit_message>
todo faq; update requirement;
</commit_message>
<xml_diff>
--- a/docs/requirement/1byone官网工作量估计v2.xlsx
+++ b/docs/requirement/1byone官网工作量估计v2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/momo/Documents/翼果科技/独立站/种子用户/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\magento相关\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31540" yWindow="1260" windowWidth="24740" windowHeight="17720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-31545" yWindow="1260" windowWidth="24735" windowHeight="17715" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="工作量估计" sheetId="2" r:id="rId1"/>
@@ -20,11 +20,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'3-7讨论新增内容及遗留'!$B$1:$I$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作量估计!$G$2:$H$2</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -2535,7 +2532,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2616,12 +2613,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2644,7 +2665,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2663,8 +2684,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2682,6 +2708,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3835,13 +3864,13 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.625" customWidth="1"/>
+    <col min="7" max="7" width="7.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:10">
       <c r="G2" t="s">
         <v>30</v>
       </c>
@@ -3849,12 +3878,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:10">
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:10">
       <c r="C4" t="s">
         <v>45</v>
       </c>
@@ -3865,12 +3894,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:10">
       <c r="C5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10">
       <c r="D6" t="s">
         <v>24</v>
       </c>
@@ -3881,12 +3910,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10">
       <c r="C7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10">
       <c r="D8" t="s">
         <v>26</v>
       </c>
@@ -3897,7 +3926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:10">
       <c r="D9" t="s">
         <v>37</v>
       </c>
@@ -3911,12 +3940,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10">
       <c r="C10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10">
       <c r="D11" t="s">
         <v>28</v>
       </c>
@@ -3930,7 +3959,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10">
       <c r="C12" t="s">
         <v>33</v>
       </c>
@@ -3941,12 +3970,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10">
       <c r="C13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10">
       <c r="D14" t="s">
         <v>35</v>
       </c>
@@ -3957,7 +3986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:10">
       <c r="D15" t="s">
         <v>36</v>
       </c>
@@ -3968,7 +3997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:10">
       <c r="C16" t="s">
         <v>43</v>
       </c>
@@ -3979,7 +4008,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10">
       <c r="C17" t="s">
         <v>42</v>
       </c>
@@ -3993,12 +4022,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:10">
       <c r="B18" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:10">
       <c r="C19" t="s">
         <v>13</v>
       </c>
@@ -4009,7 +4038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:10">
       <c r="C20" t="s">
         <v>14</v>
       </c>
@@ -4020,12 +4049,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10">
       <c r="C21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:10">
       <c r="D22" t="s">
         <v>20</v>
       </c>
@@ -4036,7 +4065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10">
       <c r="D23" t="s">
         <v>21</v>
       </c>
@@ -4047,7 +4076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10">
       <c r="D24" t="s">
         <v>22</v>
       </c>
@@ -4061,7 +4090,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:10">
       <c r="C25" t="s">
         <v>18</v>
       </c>
@@ -4072,7 +4101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:10">
       <c r="C26" t="s">
         <v>15</v>
       </c>
@@ -4083,7 +4112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:10">
       <c r="C27" t="s">
         <v>16</v>
       </c>
@@ -4094,7 +4123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10">
       <c r="C28" t="s">
         <v>17</v>
       </c>
@@ -4105,7 +4134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:10">
       <c r="C29" t="s">
         <v>38</v>
       </c>
@@ -4119,12 +4148,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10">
       <c r="B30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:10">
       <c r="C31" t="s">
         <v>6</v>
       </c>
@@ -4135,7 +4164,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10">
       <c r="C32" t="s">
         <v>7</v>
       </c>
@@ -4146,17 +4175,17 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9">
       <c r="B33" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9">
       <c r="B34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9">
       <c r="C35" t="s">
         <v>10</v>
       </c>
@@ -4167,7 +4196,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9">
       <c r="C36" t="s">
         <v>11</v>
       </c>
@@ -4178,7 +4207,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9">
       <c r="C37" t="s">
         <v>12</v>
       </c>
@@ -4189,12 +4218,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9">
       <c r="B38" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9">
       <c r="C39" t="s">
         <v>8</v>
       </c>
@@ -4205,7 +4234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9">
       <c r="C40" t="s">
         <v>15</v>
       </c>
@@ -4216,7 +4245,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9">
       <c r="C41" t="s">
         <v>16</v>
       </c>
@@ -4227,7 +4256,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9">
       <c r="C42" t="s">
         <v>17</v>
       </c>
@@ -4238,7 +4267,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9">
       <c r="C43" t="s">
         <v>9</v>
       </c>
@@ -4249,12 +4278,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9">
       <c r="B44" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:9">
       <c r="C45" t="s">
         <v>50</v>
       </c>
@@ -4265,13 +4294,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:9">
       <c r="H47">
         <f>SUM(H4:H45)*1.3</f>
         <v>98.8</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9">
       <c r="G48" t="s">
         <v>47</v>
       </c>
@@ -4283,7 +4312,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="8:8">
       <c r="H50">
         <f>H48*20000/6.2</f>
         <v>14653.318502039303</v>
@@ -4304,20 +4333,20 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="113.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="47.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="113.125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="47.625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="17.125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.625" customWidth="1"/>
+    <col min="7" max="7" width="15.125" customWidth="1"/>
     <col min="8" max="8" width="29.5" customWidth="1"/>
     <col min="9" max="9" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>95</v>
       </c>
@@ -4343,7 +4372,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30.75">
       <c r="B2" s="3" t="s">
         <v>53</v>
       </c>
@@ -4366,7 +4395,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="B3" s="2" t="s">
         <v>54</v>
       </c>
@@ -4384,7 +4413,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
@@ -4402,7 +4431,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>1</v>
       </c>
@@ -4423,7 +4452,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="B6" s="2" t="s">
         <v>67</v>
       </c>
@@ -4444,7 +4473,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="B7" s="2" t="s">
         <v>58</v>
       </c>
@@ -4462,7 +4491,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="B8" s="2" t="s">
         <v>60</v>
       </c>
@@ -4480,7 +4509,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="B9" s="3" t="s">
         <v>61</v>
       </c>
@@ -4498,7 +4527,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>1</v>
       </c>
@@ -4518,7 +4547,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4541,7 +4570,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="B12" s="3" t="s">
         <v>72</v>
       </c>
@@ -4559,7 +4588,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="B13" s="2" t="s">
         <v>75</v>
       </c>
@@ -4580,7 +4609,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="B14" s="3" t="s">
         <v>106</v>
       </c>
@@ -4601,7 +4630,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="B15" s="2" t="s">
         <v>56</v>
       </c>
@@ -4619,7 +4648,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="B16" s="2" t="s">
         <v>57</v>
       </c>
@@ -4637,7 +4666,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="57" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="45.75">
       <c r="A17">
         <v>1</v>
       </c>
@@ -4658,7 +4687,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>1</v>
       </c>
@@ -4679,7 +4708,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="B19" s="2" t="s">
         <v>73</v>
       </c>
@@ -4697,7 +4726,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>2</v>
       </c>
@@ -4718,7 +4747,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>117</v>
       </c>
@@ -4727,7 +4756,7 @@
       <c r="D21" s="3"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="B22" s="7" t="s">
         <v>111</v>
       </c>
@@ -4742,7 +4771,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="B23" s="7" t="s">
         <v>112</v>
       </c>
@@ -4750,24 +4779,24 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="B24" s="7" t="s">
         <v>113</v>
       </c>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="B25" s="7"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>126</v>
       </c>
       <c r="B26" s="7"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="B27" s="7" t="s">
         <v>134</v>
       </c>
@@ -4778,7 +4807,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="B28" s="7" t="s">
         <v>127</v>
       </c>
@@ -4792,7 +4821,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="B29" s="7" t="s">
         <v>128</v>
       </c>
@@ -4806,24 +4835,24 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="B30" s="7"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="B31" s="7"/>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="B32" s="7"/>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>2</v>
       </c>
@@ -4840,7 +4869,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>2</v>
       </c>
@@ -4857,7 +4886,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="B36" s="4" t="s">
         <v>78</v>
       </c>
@@ -4871,7 +4900,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="B37" s="4" t="s">
         <v>79</v>
       </c>
@@ -4885,7 +4914,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="B38" s="4" t="s">
         <v>80</v>
       </c>
@@ -4899,7 +4928,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="B39" s="4" t="s">
         <v>81</v>
       </c>
@@ -4913,7 +4942,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>3</v>
       </c>
@@ -4930,10 +4959,10 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -4942,7 +4971,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -4953,7 +4982,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>3</v>
       </c>
@@ -4964,7 +4993,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>5</v>
       </c>
@@ -4975,12 +5004,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="B47" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="B48" s="4" t="s">
         <v>138</v>
       </c>
@@ -5005,167 +5034,491 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P323"/>
+  <dimension ref="B1:P388"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="L419" sqref="L419"/>
+    <sheetView tabSelected="1" topLeftCell="A405" workbookViewId="0">
+      <selection activeCell="J430" sqref="J430"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="12:16" x14ac:dyDescent="0.2">
-      <c r="P1" t="s">
+    <row r="1" spans="12:16" s="8" customFormat="1">
+      <c r="P1" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="12:16" ht="45" x14ac:dyDescent="0.45">
-      <c r="L8" s="8" t="s">
+    <row r="2" spans="12:16" s="8" customFormat="1"/>
+    <row r="3" spans="12:16" s="8" customFormat="1"/>
+    <row r="4" spans="12:16" s="8" customFormat="1"/>
+    <row r="5" spans="12:16" s="8" customFormat="1"/>
+    <row r="6" spans="12:16" s="8" customFormat="1"/>
+    <row r="7" spans="12:16" s="8" customFormat="1"/>
+    <row r="8" spans="12:16" s="8" customFormat="1" ht="45">
+      <c r="L8" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="12:12" ht="45" x14ac:dyDescent="0.45">
-      <c r="L25" s="8" t="s">
+    <row r="9" spans="12:16" s="8" customFormat="1"/>
+    <row r="10" spans="12:16" s="8" customFormat="1"/>
+    <row r="11" spans="12:16" s="8" customFormat="1"/>
+    <row r="12" spans="12:16" s="8" customFormat="1"/>
+    <row r="13" spans="12:16" s="8" customFormat="1"/>
+    <row r="14" spans="12:16" s="8" customFormat="1"/>
+    <row r="15" spans="12:16" s="8" customFormat="1"/>
+    <row r="16" spans="12:16" s="8" customFormat="1"/>
+    <row r="17" spans="12:12" s="8" customFormat="1"/>
+    <row r="18" spans="12:12" s="8" customFormat="1"/>
+    <row r="21" spans="12:12" s="10" customFormat="1"/>
+    <row r="22" spans="12:12" s="10" customFormat="1"/>
+    <row r="23" spans="12:12" s="10" customFormat="1"/>
+    <row r="24" spans="12:12" s="10" customFormat="1"/>
+    <row r="25" spans="12:12" s="10" customFormat="1" ht="45">
+      <c r="L25" s="11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="12:12" ht="45" x14ac:dyDescent="0.45">
-      <c r="L32" s="8" t="s">
+    <row r="26" spans="12:12" s="10" customFormat="1"/>
+    <row r="27" spans="12:12" s="10" customFormat="1"/>
+    <row r="30" spans="12:12" s="8" customFormat="1"/>
+    <row r="31" spans="12:12" s="8" customFormat="1"/>
+    <row r="32" spans="12:12" s="8" customFormat="1" ht="45">
+      <c r="L32" s="9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="9:12" ht="45" x14ac:dyDescent="0.45">
-      <c r="L37" s="8" t="s">
+    <row r="33" spans="9:12" s="8" customFormat="1"/>
+    <row r="34" spans="9:12" s="8" customFormat="1"/>
+    <row r="35" spans="9:12" s="8" customFormat="1"/>
+    <row r="36" spans="9:12" s="8" customFormat="1"/>
+    <row r="37" spans="9:12" s="8" customFormat="1" ht="45">
+      <c r="L37" s="9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="9:12" x14ac:dyDescent="0.2">
-      <c r="I39" t="s">
+    <row r="38" spans="9:12" s="8" customFormat="1"/>
+    <row r="39" spans="9:12" s="8" customFormat="1">
+      <c r="I39" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="9:12" ht="45" x14ac:dyDescent="0.45">
-      <c r="L44" s="8" t="s">
+    <row r="40" spans="9:12" s="8" customFormat="1"/>
+    <row r="41" spans="9:12" s="8" customFormat="1"/>
+    <row r="42" spans="9:12" s="8" customFormat="1"/>
+    <row r="43" spans="9:12" s="8" customFormat="1"/>
+    <row r="44" spans="9:12" s="8" customFormat="1" ht="45">
+      <c r="L44" s="9" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H50" t="s">
+    <row r="45" spans="9:12" s="8" customFormat="1"/>
+    <row r="46" spans="9:12" s="8" customFormat="1"/>
+    <row r="47" spans="9:12" s="8" customFormat="1"/>
+    <row r="48" spans="9:12" s="8" customFormat="1"/>
+    <row r="49" spans="8:8" s="8" customFormat="1"/>
+    <row r="50" spans="8:8" s="8" customFormat="1">
+      <c r="H50" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B75" t="s">
+    <row r="51" spans="8:8" s="8" customFormat="1"/>
+    <row r="52" spans="8:8" s="8" customFormat="1"/>
+    <row r="53" spans="8:8" s="8" customFormat="1"/>
+    <row r="57" spans="8:8" s="10" customFormat="1"/>
+    <row r="58" spans="8:8" s="10" customFormat="1"/>
+    <row r="59" spans="8:8" s="10" customFormat="1"/>
+    <row r="60" spans="8:8" s="10" customFormat="1"/>
+    <row r="61" spans="8:8" s="10" customFormat="1"/>
+    <row r="62" spans="8:8" s="10" customFormat="1"/>
+    <row r="63" spans="8:8" s="10" customFormat="1"/>
+    <row r="64" spans="8:8" s="10" customFormat="1"/>
+    <row r="65" spans="2:16" s="10" customFormat="1"/>
+    <row r="66" spans="2:16" s="10" customFormat="1"/>
+    <row r="67" spans="2:16" s="10" customFormat="1"/>
+    <row r="68" spans="2:16" s="10" customFormat="1"/>
+    <row r="69" spans="2:16" s="10" customFormat="1"/>
+    <row r="70" spans="2:16" s="10" customFormat="1"/>
+    <row r="71" spans="2:16" s="10" customFormat="1"/>
+    <row r="72" spans="2:16" s="10" customFormat="1"/>
+    <row r="73" spans="2:16" s="10" customFormat="1"/>
+    <row r="74" spans="2:16" s="10" customFormat="1"/>
+    <row r="75" spans="2:16" s="10" customFormat="1">
+      <c r="B75" s="10" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="M80" t="s">
+    <row r="78" spans="2:16" s="8" customFormat="1"/>
+    <row r="79" spans="2:16" s="8" customFormat="1"/>
+    <row r="80" spans="2:16" s="8" customFormat="1">
+      <c r="M80" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="P80">
+      <c r="P80" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M85" s="9" t="s">
+    <row r="81" spans="13:13" s="8" customFormat="1"/>
+    <row r="82" spans="13:13" s="8" customFormat="1"/>
+    <row r="83" spans="13:13" s="8" customFormat="1"/>
+    <row r="84" spans="13:13" s="13" customFormat="1"/>
+    <row r="85" spans="13:13" s="8" customFormat="1">
+      <c r="M85" s="12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="88" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M88" t="s">
+    <row r="86" spans="13:13" s="8" customFormat="1"/>
+    <row r="87" spans="13:13" s="8" customFormat="1"/>
+    <row r="88" spans="13:13" s="8" customFormat="1">
+      <c r="M88" s="8" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="103" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="M103" t="s">
+    <row r="89" spans="13:13" s="8" customFormat="1"/>
+    <row r="90" spans="13:13" s="8" customFormat="1"/>
+    <row r="91" spans="13:13" s="8" customFormat="1"/>
+    <row r="94" spans="13:13" s="10" customFormat="1"/>
+    <row r="95" spans="13:13" s="10" customFormat="1"/>
+    <row r="96" spans="13:13" s="10" customFormat="1"/>
+    <row r="97" spans="13:16" s="10" customFormat="1"/>
+    <row r="98" spans="13:16" s="10" customFormat="1"/>
+    <row r="99" spans="13:16" s="10" customFormat="1"/>
+    <row r="100" spans="13:16" s="10" customFormat="1"/>
+    <row r="101" spans="13:16" s="10" customFormat="1"/>
+    <row r="102" spans="13:16" s="10" customFormat="1"/>
+    <row r="103" spans="13:16" s="10" customFormat="1">
+      <c r="M103" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="P103">
+      <c r="P103" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="M123" t="s">
+    <row r="104" spans="13:16" s="10" customFormat="1"/>
+    <row r="105" spans="13:16" s="10" customFormat="1"/>
+    <row r="106" spans="13:16" s="10" customFormat="1"/>
+    <row r="107" spans="13:16" s="10" customFormat="1"/>
+    <row r="108" spans="13:16" s="10" customFormat="1"/>
+    <row r="109" spans="13:16" s="10" customFormat="1"/>
+    <row r="110" spans="13:16" s="10" customFormat="1"/>
+    <row r="114" spans="13:16" s="14" customFormat="1"/>
+    <row r="115" spans="13:16" s="14" customFormat="1"/>
+    <row r="116" spans="13:16" s="14" customFormat="1"/>
+    <row r="117" spans="13:16" s="14" customFormat="1"/>
+    <row r="118" spans="13:16" s="14" customFormat="1"/>
+    <row r="119" spans="13:16" s="14" customFormat="1"/>
+    <row r="120" spans="13:16" s="14" customFormat="1"/>
+    <row r="121" spans="13:16" s="14" customFormat="1"/>
+    <row r="122" spans="13:16" s="14" customFormat="1"/>
+    <row r="123" spans="13:16" s="14" customFormat="1">
+      <c r="M123" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P123">
+      <c r="P123" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="M148" t="s">
+    <row r="124" spans="13:16" s="14" customFormat="1"/>
+    <row r="125" spans="13:16" s="14" customFormat="1"/>
+    <row r="126" spans="13:16" s="14" customFormat="1"/>
+    <row r="127" spans="13:16" s="14" customFormat="1"/>
+    <row r="128" spans="13:16" s="14" customFormat="1"/>
+    <row r="129" s="14" customFormat="1"/>
+    <row r="130" s="14" customFormat="1"/>
+    <row r="131" s="14" customFormat="1"/>
+    <row r="132" s="14" customFormat="1"/>
+    <row r="133" s="14" customFormat="1"/>
+    <row r="134" s="14" customFormat="1"/>
+    <row r="135" s="14" customFormat="1"/>
+    <row r="136" s="14" customFormat="1"/>
+    <row r="137" s="14" customFormat="1"/>
+    <row r="138" s="14" customFormat="1"/>
+    <row r="139" s="14" customFormat="1"/>
+    <row r="140" s="14" customFormat="1"/>
+    <row r="141" s="14" customFormat="1"/>
+    <row r="142" s="14" customFormat="1"/>
+    <row r="143" s="14" customFormat="1"/>
+    <row r="144" s="14" customFormat="1"/>
+    <row r="145" spans="13:16" s="14" customFormat="1"/>
+    <row r="146" spans="13:16" s="14" customFormat="1"/>
+    <row r="147" spans="13:16" s="14" customFormat="1"/>
+    <row r="148" spans="13:16" s="14" customFormat="1">
+      <c r="M148" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P148">
+      <c r="P148" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="M175" t="s">
+    <row r="149" spans="13:16" s="14" customFormat="1"/>
+    <row r="150" spans="13:16" s="14" customFormat="1"/>
+    <row r="151" spans="13:16" s="14" customFormat="1"/>
+    <row r="152" spans="13:16" s="14" customFormat="1"/>
+    <row r="153" spans="13:16" s="14" customFormat="1"/>
+    <row r="154" spans="13:16" s="14" customFormat="1"/>
+    <row r="155" spans="13:16" s="14" customFormat="1"/>
+    <row r="156" spans="13:16" s="14" customFormat="1"/>
+    <row r="157" spans="13:16" s="14" customFormat="1"/>
+    <row r="158" spans="13:16" s="14" customFormat="1"/>
+    <row r="159" spans="13:16" s="14" customFormat="1"/>
+    <row r="160" spans="13:16" s="14" customFormat="1"/>
+    <row r="164" spans="13:16" s="10" customFormat="1"/>
+    <row r="165" spans="13:16" s="10" customFormat="1"/>
+    <row r="166" spans="13:16" s="10" customFormat="1"/>
+    <row r="167" spans="13:16" s="10" customFormat="1"/>
+    <row r="168" spans="13:16" s="10" customFormat="1"/>
+    <row r="169" spans="13:16" s="10" customFormat="1"/>
+    <row r="170" spans="13:16" s="10" customFormat="1"/>
+    <row r="171" spans="13:16" s="10" customFormat="1"/>
+    <row r="172" spans="13:16" s="10" customFormat="1"/>
+    <row r="173" spans="13:16" s="10" customFormat="1"/>
+    <row r="174" spans="13:16" s="10" customFormat="1"/>
+    <row r="175" spans="13:16" s="10" customFormat="1">
+      <c r="M175" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="P175">
+      <c r="P175" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L201" t="s">
+    <row r="176" spans="13:16" s="10" customFormat="1"/>
+    <row r="177" s="10" customFormat="1"/>
+    <row r="178" s="10" customFormat="1"/>
+    <row r="179" s="10" customFormat="1"/>
+    <row r="180" s="10" customFormat="1"/>
+    <row r="181" s="10" customFormat="1"/>
+    <row r="182" s="10" customFormat="1"/>
+    <row r="183" s="10" customFormat="1"/>
+    <row r="184" s="10" customFormat="1"/>
+    <row r="185" s="10" customFormat="1"/>
+    <row r="186" s="10" customFormat="1"/>
+    <row r="187" s="10" customFormat="1"/>
+    <row r="188" s="10" customFormat="1"/>
+    <row r="189" s="10" customFormat="1"/>
+    <row r="193" spans="12:12" s="8" customFormat="1"/>
+    <row r="194" spans="12:12" s="8" customFormat="1"/>
+    <row r="195" spans="12:12" s="8" customFormat="1"/>
+    <row r="196" spans="12:12" s="8" customFormat="1"/>
+    <row r="197" spans="12:12" s="8" customFormat="1"/>
+    <row r="198" spans="12:12" s="8" customFormat="1"/>
+    <row r="199" spans="12:12" s="8" customFormat="1"/>
+    <row r="200" spans="12:12" s="8" customFormat="1"/>
+    <row r="201" spans="12:12" s="8" customFormat="1">
+      <c r="L201" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="223" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L223" t="s">
+    <row r="202" spans="12:12" s="8" customFormat="1"/>
+    <row r="203" spans="12:12" s="8" customFormat="1"/>
+    <row r="204" spans="12:12" s="8" customFormat="1"/>
+    <row r="205" spans="12:12" s="8" customFormat="1"/>
+    <row r="206" spans="12:12" s="8" customFormat="1"/>
+    <row r="207" spans="12:12" s="8" customFormat="1"/>
+    <row r="212" spans="12:12" s="8" customFormat="1"/>
+    <row r="213" spans="12:12" s="8" customFormat="1"/>
+    <row r="214" spans="12:12" s="8" customFormat="1"/>
+    <row r="215" spans="12:12" s="8" customFormat="1"/>
+    <row r="216" spans="12:12" s="8" customFormat="1"/>
+    <row r="217" spans="12:12" s="8" customFormat="1"/>
+    <row r="218" spans="12:12" s="8" customFormat="1"/>
+    <row r="219" spans="12:12" s="8" customFormat="1"/>
+    <row r="220" spans="12:12" s="8" customFormat="1"/>
+    <row r="221" spans="12:12" s="8" customFormat="1"/>
+    <row r="222" spans="12:12" s="8" customFormat="1"/>
+    <row r="223" spans="12:12" s="8" customFormat="1">
+      <c r="L223" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="242" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B242" t="s">
+    <row r="224" spans="12:12" s="8" customFormat="1"/>
+    <row r="225" s="8" customFormat="1"/>
+    <row r="226" s="8" customFormat="1"/>
+    <row r="227" s="8" customFormat="1"/>
+    <row r="228" s="8" customFormat="1"/>
+    <row r="229" s="8" customFormat="1"/>
+    <row r="230" s="8" customFormat="1"/>
+    <row r="231" s="8" customFormat="1"/>
+    <row r="232" s="8" customFormat="1"/>
+    <row r="233" s="8" customFormat="1"/>
+    <row r="234" s="8" customFormat="1"/>
+    <row r="235" s="8" customFormat="1"/>
+    <row r="236" s="8" customFormat="1"/>
+    <row r="237" s="8" customFormat="1"/>
+    <row r="238" s="8" customFormat="1"/>
+    <row r="239" s="8" customFormat="1"/>
+    <row r="242" spans="2:16" s="10" customFormat="1">
+      <c r="B242" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="246" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L246" t="s">
+    <row r="243" spans="2:16" s="10" customFormat="1"/>
+    <row r="244" spans="2:16" s="10" customFormat="1"/>
+    <row r="245" spans="2:16" s="10" customFormat="1"/>
+    <row r="246" spans="2:16" s="10" customFormat="1">
+      <c r="L246" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="P246">
+      <c r="P246" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="12:16" x14ac:dyDescent="0.2">
-      <c r="L259" t="s">
+    <row r="247" spans="2:16" s="10" customFormat="1"/>
+    <row r="248" spans="2:16" s="10" customFormat="1"/>
+    <row r="249" spans="2:16" s="10" customFormat="1"/>
+    <row r="252" spans="2:16" s="8" customFormat="1"/>
+    <row r="253" spans="2:16" s="8" customFormat="1"/>
+    <row r="254" spans="2:16" s="8" customFormat="1"/>
+    <row r="255" spans="2:16" s="8" customFormat="1"/>
+    <row r="256" spans="2:16" s="8" customFormat="1"/>
+    <row r="257" spans="12:16" s="8" customFormat="1"/>
+    <row r="258" spans="12:16" s="8" customFormat="1"/>
+    <row r="259" spans="12:16" s="8" customFormat="1">
+      <c r="L259" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="P259">
+      <c r="P259" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="281" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="M281" t="s">
+    <row r="260" spans="12:16" s="8" customFormat="1"/>
+    <row r="261" spans="12:16" s="8" customFormat="1"/>
+    <row r="262" spans="12:16" s="8" customFormat="1"/>
+    <row r="263" spans="12:16" s="8" customFormat="1"/>
+    <row r="264" spans="12:16" s="8" customFormat="1"/>
+    <row r="265" spans="12:16" s="8" customFormat="1"/>
+    <row r="266" spans="12:16" s="8" customFormat="1"/>
+    <row r="267" spans="12:16" s="8" customFormat="1"/>
+    <row r="268" spans="12:16" s="8" customFormat="1"/>
+    <row r="269" spans="12:16" s="8" customFormat="1"/>
+    <row r="270" spans="12:16" s="8" customFormat="1"/>
+    <row r="271" spans="12:16" s="8" customFormat="1"/>
+    <row r="272" spans="12:16" s="8" customFormat="1"/>
+    <row r="273" spans="13:16" s="8" customFormat="1"/>
+    <row r="274" spans="13:16" s="8" customFormat="1"/>
+    <row r="275" spans="13:16" s="8" customFormat="1"/>
+    <row r="276" spans="13:16" s="8" customFormat="1"/>
+    <row r="277" spans="13:16" s="8" customFormat="1"/>
+    <row r="278" spans="13:16" s="8" customFormat="1"/>
+    <row r="279" spans="13:16" s="8" customFormat="1"/>
+    <row r="280" spans="13:16" s="8" customFormat="1"/>
+    <row r="281" spans="13:16" s="8" customFormat="1">
+      <c r="M281" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="P281">
+      <c r="P281" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="M305" t="s">
+    <row r="282" spans="13:16" s="8" customFormat="1"/>
+    <row r="283" spans="13:16" s="8" customFormat="1"/>
+    <row r="284" spans="13:16" s="8" customFormat="1"/>
+    <row r="285" spans="13:16" s="8" customFormat="1"/>
+    <row r="286" spans="13:16" s="8" customFormat="1"/>
+    <row r="287" spans="13:16" s="8" customFormat="1"/>
+    <row r="288" spans="13:16" s="8" customFormat="1"/>
+    <row r="289" s="8" customFormat="1"/>
+    <row r="290" s="8" customFormat="1"/>
+    <row r="291" s="8" customFormat="1"/>
+    <row r="292" s="8" customFormat="1"/>
+    <row r="293" s="8" customFormat="1"/>
+    <row r="294" s="8" customFormat="1"/>
+    <row r="297" s="10" customFormat="1"/>
+    <row r="302" s="10" customFormat="1"/>
+    <row r="303" s="10" customFormat="1"/>
+    <row r="304" s="10" customFormat="1"/>
+    <row r="305" spans="13:16" s="10" customFormat="1">
+      <c r="M305" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="P305">
+      <c r="P305" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="13:16" x14ac:dyDescent="0.2">
-      <c r="M323" t="s">
+    <row r="306" spans="13:16" s="10" customFormat="1"/>
+    <row r="307" spans="13:16" s="10" customFormat="1"/>
+    <row r="308" spans="13:16" s="10" customFormat="1"/>
+    <row r="309" spans="13:16" s="10" customFormat="1"/>
+    <row r="315" spans="13:16" s="10" customFormat="1"/>
+    <row r="316" spans="13:16" s="10" customFormat="1"/>
+    <row r="317" spans="13:16" s="10" customFormat="1"/>
+    <row r="318" spans="13:16" s="10" customFormat="1"/>
+    <row r="319" spans="13:16" s="10" customFormat="1"/>
+    <row r="320" spans="13:16" s="10" customFormat="1"/>
+    <row r="321" spans="13:16" s="10" customFormat="1"/>
+    <row r="322" spans="13:16" s="10" customFormat="1"/>
+    <row r="323" spans="13:16" s="10" customFormat="1">
+      <c r="M323" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="P323">
+      <c r="P323" s="10">
         <v>3</v>
       </c>
     </row>
+    <row r="324" spans="13:16" s="10" customFormat="1"/>
+    <row r="325" spans="13:16" s="10" customFormat="1"/>
+    <row r="326" spans="13:16" s="10" customFormat="1"/>
+    <row r="327" spans="13:16" s="10" customFormat="1"/>
+    <row r="328" spans="13:16" s="10" customFormat="1"/>
+    <row r="329" spans="13:16" s="10" customFormat="1"/>
+    <row r="330" spans="13:16" s="10" customFormat="1"/>
+    <row r="331" spans="13:16" s="10" customFormat="1"/>
+    <row r="332" spans="13:16" s="10" customFormat="1"/>
+    <row r="333" spans="13:16" s="10" customFormat="1"/>
+    <row r="334" spans="13:16" s="10" customFormat="1"/>
+    <row r="335" spans="13:16" s="10" customFormat="1"/>
+    <row r="336" spans="13:16" s="10" customFormat="1"/>
+    <row r="337" s="10" customFormat="1"/>
+    <row r="338" s="10" customFormat="1"/>
+    <row r="339" s="10" customFormat="1"/>
+    <row r="342" s="10" customFormat="1"/>
+    <row r="343" s="10" customFormat="1"/>
+    <row r="344" s="10" customFormat="1"/>
+    <row r="345" s="10" customFormat="1"/>
+    <row r="346" s="10" customFormat="1"/>
+    <row r="347" s="10" customFormat="1"/>
+    <row r="348" s="10" customFormat="1"/>
+    <row r="349" s="10" customFormat="1"/>
+    <row r="350" s="10" customFormat="1"/>
+    <row r="351" s="10" customFormat="1"/>
+    <row r="352" s="10" customFormat="1"/>
+    <row r="353" s="10" customFormat="1"/>
+    <row r="354" s="10" customFormat="1"/>
+    <row r="355" s="10" customFormat="1"/>
+    <row r="356" s="10" customFormat="1"/>
+    <row r="357" s="10" customFormat="1"/>
+    <row r="358" s="10" customFormat="1"/>
+    <row r="359" s="10" customFormat="1"/>
+    <row r="360" s="10" customFormat="1"/>
+    <row r="361" s="10" customFormat="1"/>
+    <row r="362" s="10" customFormat="1"/>
+    <row r="363" s="10" customFormat="1"/>
+    <row r="364" s="10" customFormat="1"/>
+    <row r="365" s="10" customFormat="1"/>
+    <row r="366" s="10" customFormat="1"/>
+    <row r="367" s="10" customFormat="1"/>
+    <row r="368" s="10" customFormat="1"/>
+    <row r="369" s="10" customFormat="1"/>
+    <row r="370" s="10" customFormat="1"/>
+    <row r="371" s="10" customFormat="1"/>
+    <row r="372" s="8" customFormat="1"/>
+    <row r="373" s="8" customFormat="1"/>
+    <row r="374" s="8" customFormat="1"/>
+    <row r="375" s="8" customFormat="1"/>
+    <row r="376" s="8" customFormat="1"/>
+    <row r="377" s="8" customFormat="1"/>
+    <row r="378" s="8" customFormat="1"/>
+    <row r="379" s="8" customFormat="1"/>
+    <row r="380" s="8" customFormat="1"/>
+    <row r="381" s="8" customFormat="1"/>
+    <row r="382" s="8" customFormat="1"/>
+    <row r="383" s="8" customFormat="1"/>
+    <row r="384" s="8" customFormat="1"/>
+    <row r="385" s="8" customFormat="1"/>
+    <row r="386" s="8" customFormat="1"/>
+    <row r="387" s="8" customFormat="1"/>
+    <row r="388" s="8" customFormat="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>